<commit_message>
added new DDD and pneumonia data
</commit_message>
<xml_diff>
--- a/DataSheet_cddep.xlsx
+++ b/DataSheet_cddep.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Yale\Galvani Lab\AMR\Carbapenem-Resistance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amber\Documents\Carbapenem\Carbapenem-Resistance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="3730" tabRatio="993" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="3735" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="United States" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,10 @@
     <sheet name="Iceland" sheetId="32" r:id="rId33"/>
     <sheet name="Malta" sheetId="33" r:id="rId34"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <externalReferences>
+    <externalReference r:id="rId35"/>
+  </externalReferences>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -170,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -440,6 +443,71 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Pneumonia"/>
+      <sheetName val="Data &amp; Parameters"/>
+      <sheetName val="Sources &amp; Notes"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="13">
+          <cell r="B13">
+            <v>5.116795146E-2</v>
+          </cell>
+          <cell r="C13">
+            <v>5.545251382E-2</v>
+          </cell>
+          <cell r="D13">
+            <v>6.4058763709999994E-2</v>
+          </cell>
+          <cell r="E13">
+            <v>6.3038341819999996E-2</v>
+          </cell>
+          <cell r="F13">
+            <v>6.9081833790000005E-2</v>
+          </cell>
+          <cell r="G13">
+            <v>7.2866838119999999E-2</v>
+          </cell>
+          <cell r="H13">
+            <v>8.1495325930000001E-2</v>
+          </cell>
+          <cell r="I13">
+            <v>8.2100477039999994E-2</v>
+          </cell>
+          <cell r="J13">
+            <v>8.4872943630000003E-2</v>
+          </cell>
+          <cell r="K13">
+            <v>8.1556849720000005E-2</v>
+          </cell>
+          <cell r="L13">
+            <v>9.3080891629999996E-2</v>
+          </cell>
+          <cell r="M13">
+            <v>9.1138155499999998E-2</v>
+          </cell>
+          <cell r="N13">
+            <v>9.7227641840000004E-2</v>
+          </cell>
+          <cell r="O13">
+            <v>9.4034273060000007E-2</v>
+          </cell>
+          <cell r="P13">
+            <v>9.8938662489999996E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,13 +782,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1"/>
-    <col min="2" max="1025" width="8.453125" style="1"/>
+    <col min="2" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,7 +832,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -808,7 +876,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -852,7 +920,7 @@
         <v>117.3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -896,7 +964,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -940,7 +1008,7 @@
         <v>153.75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -984,7 +1052,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1096,7 @@
         <v>70.09</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1140,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1154,7 @@
         <v>0.17544000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1108,14 +1176,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1233,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1270,7 +1338,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1424,14 +1492,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1549,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1546,7 +1614,7 @@
         <v>4.1843971631205677E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1586,7 +1654,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1626,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1676,7 +1744,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1740,15 +1808,15 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="2"/>
-    <col min="2" max="11" width="8.54296875" style="1"/>
-    <col min="12" max="1019" width="8.453125" style="1"/>
-    <col min="1020" max="1025" width="8.453125"/>
+    <col min="1" max="1" width="16.140625" style="2"/>
+    <col min="2" max="11" width="8.5703125" style="1"/>
+    <col min="12" max="1019" width="8.42578125" style="1"/>
+    <col min="1020" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1851,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1828,7 +1896,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1863,7 +1931,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1898,7 +1966,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1933,7 +2001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1982,14 +2050,14 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2107,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2104,7 +2172,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -2144,7 +2212,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2184,7 +2252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -2234,7 +2302,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2301,17 +2369,17 @@
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="1"/>
-    <col min="3" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="14" width="8.54296875" style="1"/>
-    <col min="15" max="1022" width="8.453125" style="1"/>
-    <col min="1023" max="1028" width="8.453125"/>
+    <col min="1" max="1" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1"/>
+    <col min="3" max="5" width="8.7109375" style="1"/>
+    <col min="6" max="14" width="8.5703125" style="1"/>
+    <col min="15" max="1022" width="8.42578125" style="1"/>
+    <col min="1023" max="1028" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1022" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2346,7 +2414,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2387,7 +2455,7 @@
       <c r="AMG2"/>
       <c r="AMH2"/>
     </row>
-    <row r="3" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +2496,7 @@
       <c r="AMG3"/>
       <c r="AMH3"/>
     </row>
-    <row r="4" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2537,7 @@
       <c r="AMG4"/>
       <c r="AMH4"/>
     </row>
-    <row r="5" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -2510,7 +2578,7 @@
       <c r="AMG5"/>
       <c r="AMH5"/>
     </row>
-    <row r="6" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -2551,7 +2619,7 @@
       <c r="AMG6"/>
       <c r="AMH6"/>
     </row>
-    <row r="7" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
@@ -2592,7 +2660,7 @@
       <c r="AMG7"/>
       <c r="AMH7"/>
     </row>
-    <row r="8" spans="1:1022" s="24" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1022" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -3632,7 +3700,7 @@
       <c r="AMA8" s="23"/>
       <c r="AMB8" s="23"/>
     </row>
-    <row r="9" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -3675,22 +3743,22 @@
       <c r="AMG9"/>
       <c r="AMH9"/>
     </row>
-    <row r="10" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -3719,7 +3787,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="17" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -3744,7 +3812,7 @@
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
     </row>
-    <row r="18" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -3769,7 +3837,7 @@
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
     </row>
-    <row r="19" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>24</v>
       </c>
@@ -3794,7 +3862,7 @@
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
     </row>
-    <row r="20" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
@@ -3826,28 +3894,28 @@
       <c r="AMG20"/>
       <c r="AMH20"/>
     </row>
-    <row r="21" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="AMF21"/>
       <c r="AMG21"/>
       <c r="AMH21"/>
     </row>
-    <row r="24" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1022" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>30</v>
       </c>
@@ -3866,14 +3934,14 @@
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3923,7 +3991,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3988,7 +4056,7 @@
         <v>4.422781839516202E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4028,7 +4096,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -4068,7 +4136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4186,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -4182,16 +4250,16 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="2" width="11.81640625"/>
-    <col min="3" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="2" width="11.85546875"/>
+    <col min="3" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4309,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -4306,7 +4374,7 @@
         <v>2.0918025022694082E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4341,7 +4409,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -4376,7 +4444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -4426,7 +4494,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -4493,14 +4561,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" style="2" customWidth="1"/>
-    <col min="2" max="15" width="8.54296875" style="1"/>
-    <col min="16" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="36.85546875" style="2" customWidth="1"/>
+    <col min="2" max="15" width="8.5703125" style="1"/>
+    <col min="16" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4532,7 +4600,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4574,7 +4642,7 @@
       <c r="AMJ2"/>
       <c r="AMK2"/>
     </row>
-    <row r="3" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -4616,7 +4684,7 @@
       <c r="AMJ3"/>
       <c r="AMK3"/>
     </row>
-    <row r="4" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -4658,7 +4726,7 @@
       <c r="AMJ4"/>
       <c r="AMK4"/>
     </row>
-    <row r="5" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
@@ -4700,7 +4768,7 @@
       <c r="AMJ5"/>
       <c r="AMK5"/>
     </row>
-    <row r="6" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
@@ -4740,7 +4808,7 @@
       <c r="AMJ6"/>
       <c r="AMK6"/>
     </row>
-    <row r="7" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
@@ -4780,7 +4848,7 @@
       <c r="AMJ7"/>
       <c r="AMK7"/>
     </row>
-    <row r="8" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -4824,7 +4892,7 @@
       <c r="AMJ8"/>
       <c r="AMK8"/>
     </row>
-    <row r="9" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -4864,7 +4932,7 @@
       <c r="AMJ9"/>
       <c r="AMK9"/>
     </row>
-    <row r="10" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
@@ -4890,7 +4958,7 @@
       <c r="AMJ10"/>
       <c r="AMK10"/>
     </row>
-    <row r="11" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
@@ -4916,7 +4984,7 @@
       <c r="AMJ11"/>
       <c r="AMK11"/>
     </row>
-    <row r="13" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
@@ -4924,7 +4992,7 @@
       <c r="F13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
@@ -4947,7 +5015,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="15" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
@@ -4970,22 +5038,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>30</v>
       </c>
@@ -5004,15 +5072,15 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5062,7 +5130,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -5127,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -5160,7 +5228,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -5193,7 +5261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -5243,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -5293,10 +5361,10 @@
         <v>8319</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -5315,15 +5383,15 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5373,7 +5441,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -6446,7 +6514,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -6478,7 +6546,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -6510,7 +6578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -6560,7 +6628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -6620,18 +6688,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="1025" width="9.1796875" style="23"/>
-    <col min="1026" max="16384" width="8.7265625" style="24"/>
+    <col min="1" max="1" width="31.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="1025" width="9.140625" style="23" customWidth="1"/>
+    <col min="1026" max="16384" width="8.7109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1025" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -6681,7 +6749,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -6731,7 +6799,7 @@
         <v>6395</v>
       </c>
     </row>
-    <row r="3" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -6783,7 +6851,7 @@
         <v>511.6</v>
       </c>
     </row>
-    <row r="4" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
@@ -6833,7 +6901,7 @@
         <v>6578</v>
       </c>
     </row>
-    <row r="5" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
@@ -6885,7 +6953,7 @@
         <v>1249.82</v>
       </c>
     </row>
-    <row r="6" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>5</v>
       </c>
@@ -6935,7 +7003,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="7" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
@@ -6987,7 +7055,7 @@
         <v>361.62</v>
       </c>
     </row>
-    <row r="8" spans="1:1025" s="32" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1025" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>34</v>
       </c>
@@ -8045,7 +8113,7 @@
       <c r="AMJ8" s="33"/>
       <c r="AMK8" s="33"/>
     </row>
-    <row r="9" spans="1:1025" s="35" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1025" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>35</v>
       </c>
@@ -9109,7 +9177,7 @@
       <c r="AMJ9" s="36"/>
       <c r="AMK9" s="36"/>
     </row>
-    <row r="10" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>7</v>
       </c>
@@ -9159,7 +9227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
@@ -9176,7 +9244,7 @@
         <v>0.1071428571</v>
       </c>
     </row>
-    <row r="12" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>9</v>
       </c>
@@ -9184,54 +9252,69 @@
         <v>0.18589</v>
       </c>
     </row>
-    <row r="13" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="23">
-        <v>4.8889240219999998E-2</v>
+        <f>'[1]Data &amp; Parameters'!$B$13</f>
+        <v>5.116795146E-2</v>
       </c>
       <c r="C13" s="23">
-        <v>5.8192576849999997E-2</v>
+        <f>'[1]Data &amp; Parameters'!$C$13</f>
+        <v>5.545251382E-2</v>
       </c>
       <c r="D13" s="23">
-        <v>7.1193937590000006E-2</v>
+        <f>'[1]Data &amp; Parameters'!$D$13</f>
+        <v>6.4058763709999994E-2</v>
       </c>
       <c r="E13" s="23">
-        <v>7.3603685429999996E-2</v>
+        <f>'[1]Data &amp; Parameters'!$E$13</f>
+        <v>6.3038341819999996E-2</v>
       </c>
       <c r="F13" s="23">
-        <v>7.9723747710000001E-2</v>
+        <f>'[1]Data &amp; Parameters'!$F$13</f>
+        <v>6.9081833790000005E-2</v>
       </c>
       <c r="G13" s="23">
-        <v>8.7776693350000004E-2</v>
+        <f>'[1]Data &amp; Parameters'!$G$13</f>
+        <v>7.2866838119999999E-2</v>
       </c>
       <c r="H13" s="23">
-        <v>9.7859175019999994E-2</v>
+        <f>'[1]Data &amp; Parameters'!$H$13</f>
+        <v>8.1495325930000001E-2</v>
       </c>
       <c r="I13" s="23">
-        <v>0.1025223968</v>
+        <f>'[1]Data &amp; Parameters'!$I$13</f>
+        <v>8.2100477039999994E-2</v>
       </c>
       <c r="J13" s="23">
-        <v>0.11102375539999999</v>
+        <f>'[1]Data &amp; Parameters'!$J$13</f>
+        <v>8.4872943630000003E-2</v>
       </c>
       <c r="K13" s="23">
-        <v>0.11769630790000001</v>
+        <f>'[1]Data &amp; Parameters'!$K$13</f>
+        <v>8.1556849720000005E-2</v>
       </c>
       <c r="L13" s="23">
-        <v>0.12059862740000001</v>
+        <f>'[1]Data &amp; Parameters'!$L$13</f>
+        <v>9.3080891629999996E-2</v>
       </c>
       <c r="M13" s="23">
-        <v>0.1273101734</v>
+        <f>'[1]Data &amp; Parameters'!$M$13</f>
+        <v>9.1138155499999998E-2</v>
       </c>
       <c r="N13" s="23">
-        <v>0.13022742849999999</v>
+        <f>'[1]Data &amp; Parameters'!$N$13</f>
+        <v>9.7227641840000004E-2</v>
       </c>
       <c r="O13" s="25">
-        <v>0.1194428094</v>
+        <f>'[1]Data &amp; Parameters'!$O$13</f>
+        <v>9.4034273060000007E-2</v>
       </c>
       <c r="P13" s="25">
-        <v>0.1262992208</v>
+        <f>'[1]Data &amp; Parameters'!$P$13</f>
+        <v>9.8938662489999996E-2</v>
       </c>
     </row>
   </sheetData>
@@ -9251,15 +9334,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10317,7 +10400,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -11390,7 +11473,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -11422,7 +11505,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -11454,7 +11537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -11504,7 +11587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -11568,15 +11651,15 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -11626,7 +11709,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -11686,7 +11769,7 @@
         <v>2.2514839325919354E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -11721,7 +11804,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -11756,7 +11839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -11806,7 +11889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -11873,13 +11956,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="1022" width="8.453125" style="1"/>
+    <col min="1" max="1" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="1022" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -11926,7 +12009,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -11975,7 +12058,7 @@
       <c r="AMG2"/>
       <c r="AMH2"/>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -12024,7 +12107,7 @@
       <c r="AMG3"/>
       <c r="AMH3"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -12073,7 +12156,7 @@
       <c r="AMG4"/>
       <c r="AMH4"/>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
@@ -12122,7 +12205,7 @@
       <c r="AMG5"/>
       <c r="AMH5"/>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
@@ -12171,7 +12254,7 @@
       <c r="AMG6"/>
       <c r="AMH6"/>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
@@ -12220,7 +12303,7 @@
       <c r="AMG7"/>
       <c r="AMH7"/>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
@@ -12271,7 +12354,7 @@
       <c r="AMG8"/>
       <c r="AMH8"/>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>8</v>
       </c>
@@ -12298,7 +12381,7 @@
       <c r="AMG9"/>
       <c r="AMH9"/>
     </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
@@ -12319,7 +12402,7 @@
       <c r="AMG10"/>
       <c r="AMH10"/>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="AMI11" s="1"/>
       <c r="AMJ11" s="1"/>
     </row>
@@ -12337,15 +12420,15 @@
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12395,7 +12478,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -12460,7 +12543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -12493,7 +12576,7 @@
       </c>
       <c r="P3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -12526,7 +12609,7 @@
       </c>
       <c r="P4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -12576,7 +12659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -12640,14 +12723,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -12697,7 +12780,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -12762,7 +12845,7 @@
         <v>8.1076418837329658E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -12798,7 +12881,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -12834,7 +12917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -12884,7 +12967,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -12948,15 +13031,15 @@
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13006,7 +13089,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -13071,7 +13154,7 @@
         <v>7.3943987429522135E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -13106,7 +13189,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -13141,7 +13224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -13191,7 +13274,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -13255,14 +13338,14 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13312,7 +13395,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -13377,7 +13460,7 @@
         <v>1.5139499675582151E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -13405,7 +13488,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -13433,7 +13516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -13483,7 +13566,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -13547,14 +13630,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="1"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="1"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13604,7 +13687,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -13669,7 +13752,7 @@
         <v>3.7306472673008769E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -13709,7 +13792,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -13749,7 +13832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -13799,7 +13882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -13863,15 +13946,15 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="1"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="8.42578125" style="1"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -14929,7 +15012,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -16002,7 +16085,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -16037,7 +16120,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -16072,7 +16155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -16122,7 +16205,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -16186,15 +16269,15 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16244,7 +16327,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -16309,7 +16392,7 @@
         <v>5.6581874455943516E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -16344,7 +16427,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -16379,7 +16462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -16429,7 +16512,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -16493,13 +16576,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="2"/>
-    <col min="2" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="16.42578125" style="2"/>
+    <col min="2" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16549,7 +16632,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -16614,7 +16697,7 @@
         <v>1.0201135598113753E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -16654,7 +16737,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -16694,7 +16777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -16744,7 +16827,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -16794,16 +16877,16 @@
         <v>10391</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -16829,15 +16912,15 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="10.7265625" style="1"/>
+    <col min="1" max="1" width="36.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -16872,7 +16955,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -16916,7 +16999,7 @@
       <c r="AMJ2"/>
       <c r="AMK2"/>
     </row>
-    <row r="3" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
@@ -16960,7 +17043,7 @@
       <c r="AMJ3"/>
       <c r="AMK3"/>
     </row>
-    <row r="4" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -17004,7 +17087,7 @@
       <c r="AMJ4"/>
       <c r="AMK4"/>
     </row>
-    <row r="5" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
@@ -17048,7 +17131,7 @@
       <c r="AMJ5"/>
       <c r="AMK5"/>
     </row>
-    <row r="6" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
@@ -17090,7 +17173,7 @@
       <c r="AMJ6"/>
       <c r="AMK6"/>
     </row>
-    <row r="7" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
@@ -17132,7 +17215,7 @@
       <c r="AMJ7"/>
       <c r="AMK7"/>
     </row>
-    <row r="8" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -17178,7 +17261,7 @@
       <c r="AMJ8"/>
       <c r="AMK8"/>
     </row>
-    <row r="9" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>8</v>
       </c>
@@ -17204,7 +17287,7 @@
       <c r="AMJ9"/>
       <c r="AMK9"/>
     </row>
-    <row r="10" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
@@ -17230,7 +17313,7 @@
       <c r="AMJ10"/>
       <c r="AMK10"/>
     </row>
-    <row r="14" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1025" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>0</v>
       </c>
@@ -17260,7 +17343,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
     </row>
-    <row r="15" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
@@ -17286,7 +17369,7 @@
       <c r="AMJ15"/>
       <c r="AMK15"/>
     </row>
-    <row r="16" spans="1:1025" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
@@ -17298,27 +17381,27 @@
       <c r="O16"/>
       <c r="P16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
     </row>
   </sheetData>
@@ -17339,13 +17422,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.54296875" style="2"/>
-    <col min="2" max="1025" width="8.54296875" style="1"/>
+    <col min="1" max="1" width="8.5703125" style="2"/>
+    <col min="2" max="1025" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17395,7 +17478,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -17460,7 +17543,7 @@
         <v>1.2611518520248494E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -17494,7 +17577,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -17528,7 +17611,7 @@
         <v>157.88999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -17578,7 +17661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -17642,12 +17725,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.54296875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17676,7 +17759,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -17705,7 +17788,7 @@
         <v>3.3306820441439699E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -17734,7 +17817,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -17789,16 +17872,16 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="2"/>
-    <col min="2" max="5" width="8.26953125"/>
-    <col min="6" max="6" width="8.453125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="8.42578125" style="2"/>
+    <col min="2" max="5" width="8.28515625"/>
+    <col min="6" max="6" width="8.42578125"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -17848,7 +17931,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -17863,7 +17946,7 @@
       <c r="O2"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -17890,7 +17973,7 @@
       <c r="O3"/>
       <c r="P3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -17917,7 +18000,7 @@
       <c r="O4"/>
       <c r="P4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -17952,15 +18035,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -17979,12 +18062,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18019,7 +18102,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -18048,7 +18131,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -18083,7 +18166,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -18118,16 +18201,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -18146,13 +18229,13 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2"/>
-    <col min="2" max="1025" width="8.453125" style="1"/>
+    <col min="2" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18202,7 +18285,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -18267,7 +18350,7 @@
         <v>3.7487073422957599E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -18299,7 +18382,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -18331,7 +18414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -18381,7 +18464,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -18431,16 +18514,16 @@
         <v>15472</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -18459,16 +18542,16 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="2"/>
-    <col min="2" max="8" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="19.85546875" style="2"/>
+    <col min="2" max="8" width="8.7109375" style="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="10" max="16" width="8.7109375" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18518,7 +18601,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -18583,7 +18666,7 @@
         <v>1.2172854534388314E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -18623,7 +18706,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -18663,7 +18746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -18713,7 +18796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -18777,14 +18860,14 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" style="1"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="18.28515625" style="1"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18834,7 +18917,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -18894,7 +18977,7 @@
         <v>3.8319327731092439E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -18924,7 +19007,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -18954,7 +19037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -19004,7 +19087,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -19068,12 +19151,12 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19108,7 +19191,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -19141,7 +19224,7 @@
         <v>0.121</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -19176,7 +19259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -19211,21 +19294,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -19244,14 +19327,14 @@
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="2"/>
-    <col min="2" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="8.42578125" style="2"/>
+    <col min="2" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19301,7 +19384,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -19366,7 +19449,7 @@
         <v>2.7825150345570414E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -19406,7 +19489,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -19446,7 +19529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -19496,7 +19579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -19560,15 +19643,15 @@
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="2"/>
-    <col min="2" max="6" width="8.26953125"/>
-    <col min="7" max="16" width="8.54296875" style="1"/>
-    <col min="17" max="1025" width="8.453125" style="1"/>
+    <col min="1" max="1" width="8.42578125" style="2"/>
+    <col min="2" max="6" width="8.28515625"/>
+    <col min="7" max="16" width="8.5703125" style="1"/>
+    <col min="17" max="1025" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -19618,7 +19701,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -20691,7 +20774,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -20723,7 +20806,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -20755,7 +20838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -20805,7 +20888,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
sorry forgot to include this
</commit_message>
<xml_diff>
--- a/DataSheet_cddep.xlsx
+++ b/DataSheet_cddep.xlsx
@@ -47,9 +47,6 @@
     <sheet name="Iceland" sheetId="32" r:id="rId33"/>
     <sheet name="Malta" sheetId="33" r:id="rId34"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId35"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -443,71 +440,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Pneumonia"/>
-      <sheetName val="Data &amp; Parameters"/>
-      <sheetName val="Sources &amp; Notes"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="13">
-          <cell r="B13">
-            <v>5.116795146E-2</v>
-          </cell>
-          <cell r="C13">
-            <v>5.545251382E-2</v>
-          </cell>
-          <cell r="D13">
-            <v>6.4058763709999994E-2</v>
-          </cell>
-          <cell r="E13">
-            <v>6.3038341819999996E-2</v>
-          </cell>
-          <cell r="F13">
-            <v>6.9081833790000005E-2</v>
-          </cell>
-          <cell r="G13">
-            <v>7.2866838119999999E-2</v>
-          </cell>
-          <cell r="H13">
-            <v>8.1495325930000001E-2</v>
-          </cell>
-          <cell r="I13">
-            <v>8.2100477039999994E-2</v>
-          </cell>
-          <cell r="J13">
-            <v>8.4872943630000003E-2</v>
-          </cell>
-          <cell r="K13">
-            <v>8.1556849720000005E-2</v>
-          </cell>
-          <cell r="L13">
-            <v>9.3080891629999996E-2</v>
-          </cell>
-          <cell r="M13">
-            <v>9.1138155499999998E-2</v>
-          </cell>
-          <cell r="N13">
-            <v>9.7227641840000004E-2</v>
-          </cell>
-          <cell r="O13">
-            <v>9.4034273060000007E-2</v>
-          </cell>
-          <cell r="P13">
-            <v>9.8938662489999996E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6689,7 +6621,7 @@
   <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9257,63 +9189,48 @@
         <v>33</v>
       </c>
       <c r="B13" s="23">
-        <f>'[1]Data &amp; Parameters'!$B$13</f>
         <v>5.116795146E-2</v>
       </c>
       <c r="C13" s="23">
-        <f>'[1]Data &amp; Parameters'!$C$13</f>
         <v>5.545251382E-2</v>
       </c>
       <c r="D13" s="23">
-        <f>'[1]Data &amp; Parameters'!$D$13</f>
         <v>6.4058763709999994E-2</v>
       </c>
       <c r="E13" s="23">
-        <f>'[1]Data &amp; Parameters'!$E$13</f>
         <v>6.3038341819999996E-2</v>
       </c>
       <c r="F13" s="23">
-        <f>'[1]Data &amp; Parameters'!$F$13</f>
         <v>6.9081833790000005E-2</v>
       </c>
       <c r="G13" s="23">
-        <f>'[1]Data &amp; Parameters'!$G$13</f>
         <v>7.2866838119999999E-2</v>
       </c>
       <c r="H13" s="23">
-        <f>'[1]Data &amp; Parameters'!$H$13</f>
         <v>8.1495325930000001E-2</v>
       </c>
       <c r="I13" s="23">
-        <f>'[1]Data &amp; Parameters'!$I$13</f>
         <v>8.2100477039999994E-2</v>
       </c>
       <c r="J13" s="23">
-        <f>'[1]Data &amp; Parameters'!$J$13</f>
         <v>8.4872943630000003E-2</v>
       </c>
       <c r="K13" s="23">
-        <f>'[1]Data &amp; Parameters'!$K$13</f>
         <v>8.1556849720000005E-2</v>
       </c>
       <c r="L13" s="23">
-        <f>'[1]Data &amp; Parameters'!$L$13</f>
         <v>9.3080891629999996E-2</v>
       </c>
       <c r="M13" s="23">
-        <f>'[1]Data &amp; Parameters'!$M$13</f>
         <v>9.1138155499999998E-2</v>
       </c>
       <c r="N13" s="23">
-        <f>'[1]Data &amp; Parameters'!$N$13</f>
         <v>9.7227641840000004E-2</v>
       </c>
       <c r="O13" s="25">
-        <f>'[1]Data &amp; Parameters'!$O$13</f>
         <v>9.4034273060000007E-2</v>
       </c>
       <c r="P13" s="25">
-        <f>'[1]Data &amp; Parameters'!$P$13</f>
         <v>9.8938662489999996E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed parameter names and cleaned code and other changes
</commit_message>
<xml_diff>
--- a/DataSheet_cddep.xlsx
+++ b/DataSheet_cddep.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
   <si>
     <t>Year</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Resistance_EA/C</t>
+  </si>
+  <si>
+    <t>Pneumonia prevalence</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,6 +360,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6618,10 +6625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK13"/>
+  <dimension ref="A1:AMK14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,309 +6689,309 @@
       </c>
     </row>
     <row r="2" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="32">
-        <v>3230</v>
-      </c>
-      <c r="C2" s="32">
-        <v>3459</v>
-      </c>
-      <c r="D2" s="32">
-        <v>3697</v>
-      </c>
-      <c r="E2" s="32">
-        <v>3733</v>
-      </c>
-      <c r="F2" s="32">
-        <v>4616</v>
-      </c>
-      <c r="G2" s="32">
-        <v>4696</v>
-      </c>
-      <c r="H2" s="32">
-        <v>4158</v>
-      </c>
-      <c r="I2" s="32">
-        <v>3732</v>
-      </c>
-      <c r="J2" s="32">
-        <v>3745</v>
-      </c>
-      <c r="K2" s="33">
-        <v>3286</v>
-      </c>
-      <c r="L2" s="33">
-        <v>3039</v>
-      </c>
-      <c r="M2" s="33">
-        <v>2503</v>
-      </c>
-      <c r="N2" s="33">
-        <v>1173</v>
-      </c>
-      <c r="O2" s="33">
-        <v>6162</v>
-      </c>
-      <c r="P2" s="33">
-        <v>6395</v>
+      <c r="A2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="38">
+        <v>2486</v>
+      </c>
+      <c r="C2" s="38">
+        <v>2727</v>
+      </c>
+      <c r="D2" s="38">
+        <v>2822</v>
+      </c>
+      <c r="E2" s="38">
+        <v>3101</v>
+      </c>
+      <c r="F2" s="38">
+        <v>3537</v>
+      </c>
+      <c r="G2" s="38">
+        <v>3076</v>
+      </c>
+      <c r="H2" s="38">
+        <v>2714</v>
+      </c>
+      <c r="I2" s="38">
+        <v>2267</v>
+      </c>
+      <c r="J2" s="39">
+        <v>2107</v>
+      </c>
+      <c r="K2" s="39">
+        <v>1829</v>
+      </c>
+      <c r="L2" s="39">
+        <v>1631</v>
+      </c>
+      <c r="M2" s="39">
+        <v>1488</v>
+      </c>
+      <c r="N2" s="39">
+        <v>615</v>
+      </c>
+      <c r="O2" s="39">
+        <v>6849</v>
+      </c>
+      <c r="P2" s="39">
+        <v>6578</v>
       </c>
     </row>
     <row r="3" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="35">
-        <v>0</v>
+        <v>323.18</v>
       </c>
       <c r="C3" s="35">
-        <v>0</v>
+        <v>436.32</v>
       </c>
       <c r="D3" s="35">
-        <v>0</v>
+        <v>507.96</v>
       </c>
       <c r="E3" s="35">
-        <v>0</v>
+        <v>589.19000000000005</v>
       </c>
       <c r="F3" s="35">
-        <v>0</v>
+        <v>707.4</v>
       </c>
       <c r="G3" s="35">
-        <v>46.96</v>
+        <v>522.91999999999996</v>
       </c>
       <c r="H3" s="35">
-        <v>41.58</v>
+        <v>488.52</v>
       </c>
       <c r="I3" s="35">
-        <v>74.64</v>
+        <v>385.39</v>
       </c>
       <c r="J3" s="35">
-        <v>187.25</v>
-      </c>
-      <c r="K3" s="36">
-        <v>164.3</v>
-      </c>
-      <c r="L3" s="36">
-        <v>151.94999999999999</v>
-      </c>
-      <c r="M3" s="36">
-        <v>175.21</v>
-      </c>
-      <c r="N3" s="36">
-        <v>117.3</v>
+        <v>379.26</v>
+      </c>
+      <c r="K3" s="35">
+        <v>310.93</v>
+      </c>
+      <c r="L3" s="35">
+        <v>326.2</v>
+      </c>
+      <c r="M3" s="35">
+        <v>282.72000000000003</v>
+      </c>
+      <c r="N3" s="35">
+        <v>153.75</v>
       </c>
       <c r="O3" s="36">
-        <f>0.1*O2</f>
-        <v>616.20000000000005</v>
+        <f>0.2*O2</f>
+        <v>1369.8000000000002</v>
       </c>
       <c r="P3" s="36">
-        <f>0.08*P2</f>
-        <v>511.6</v>
+        <f>0.19*P2</f>
+        <v>1249.82</v>
       </c>
     </row>
     <row r="4" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="38">
-        <v>2486</v>
+        <v>681</v>
       </c>
       <c r="C4" s="38">
-        <v>2727</v>
+        <v>887</v>
       </c>
       <c r="D4" s="38">
-        <v>2822</v>
+        <v>955</v>
       </c>
       <c r="E4" s="38">
-        <v>3101</v>
+        <v>998</v>
       </c>
       <c r="F4" s="38">
-        <v>3537</v>
+        <v>1187</v>
       </c>
       <c r="G4" s="38">
-        <v>3076</v>
+        <v>1143</v>
       </c>
       <c r="H4" s="38">
-        <v>2714</v>
-      </c>
-      <c r="I4" s="38">
-        <v>2267</v>
+        <v>890</v>
+      </c>
+      <c r="I4" s="39">
+        <v>860</v>
       </c>
       <c r="J4" s="39">
-        <v>2107</v>
+        <v>757</v>
       </c>
       <c r="K4" s="39">
-        <v>1829</v>
+        <v>603</v>
       </c>
       <c r="L4" s="39">
-        <v>1631</v>
+        <v>419</v>
       </c>
       <c r="M4" s="39">
-        <v>1488</v>
+        <v>365</v>
       </c>
       <c r="N4" s="39">
-        <v>615</v>
+        <v>163</v>
       </c>
       <c r="O4" s="39">
-        <v>6849</v>
+        <v>831</v>
       </c>
       <c r="P4" s="39">
-        <v>6578</v>
+        <v>738</v>
       </c>
     </row>
     <row r="5" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="35">
-        <v>323.18</v>
-      </c>
-      <c r="C5" s="35">
-        <v>436.32</v>
-      </c>
-      <c r="D5" s="35">
-        <v>507.96</v>
-      </c>
-      <c r="E5" s="35">
-        <v>589.19000000000005</v>
-      </c>
-      <c r="F5" s="35">
-        <v>707.4</v>
-      </c>
-      <c r="G5" s="35">
-        <v>522.91999999999996</v>
-      </c>
-      <c r="H5" s="35">
-        <v>488.52</v>
-      </c>
-      <c r="I5" s="35">
-        <v>385.39</v>
-      </c>
-      <c r="J5" s="35">
-        <v>379.26</v>
-      </c>
-      <c r="K5" s="35">
-        <v>310.93</v>
-      </c>
-      <c r="L5" s="35">
-        <v>326.2</v>
-      </c>
-      <c r="M5" s="35">
-        <v>282.72000000000003</v>
-      </c>
-      <c r="N5" s="35">
-        <v>153.75</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="36">
+        <v>61.29</v>
+      </c>
+      <c r="C5" s="36">
+        <v>124.18</v>
+      </c>
+      <c r="D5" s="36">
+        <v>191</v>
+      </c>
+      <c r="E5" s="36">
+        <v>179.64</v>
+      </c>
+      <c r="F5" s="36">
+        <v>213.66</v>
+      </c>
+      <c r="G5" s="36">
+        <v>262.89</v>
+      </c>
+      <c r="H5" s="36">
+        <v>186.9</v>
+      </c>
+      <c r="I5" s="36">
+        <v>301</v>
+      </c>
+      <c r="J5" s="36">
+        <v>295.23</v>
+      </c>
+      <c r="K5" s="36">
+        <v>301.5</v>
+      </c>
+      <c r="L5" s="36">
+        <v>184.36</v>
+      </c>
+      <c r="M5" s="36">
+        <v>135.05000000000001</v>
+      </c>
+      <c r="N5" s="36">
+        <v>70.09</v>
       </c>
       <c r="O5" s="36">
-        <f>0.2*O4</f>
-        <v>1369.8000000000002</v>
+        <f>0.54*O4</f>
+        <v>448.74</v>
       </c>
       <c r="P5" s="36">
-        <f>0.19*P4</f>
-        <v>1249.82</v>
+        <f>0.49*P4</f>
+        <v>361.62</v>
       </c>
     </row>
     <row r="6" spans="1:1025" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="38">
-        <v>681</v>
-      </c>
-      <c r="C6" s="38">
-        <v>887</v>
-      </c>
-      <c r="D6" s="38">
-        <v>955</v>
-      </c>
-      <c r="E6" s="38">
-        <v>998</v>
-      </c>
-      <c r="F6" s="38">
-        <v>1187</v>
-      </c>
-      <c r="G6" s="38">
-        <v>1143</v>
-      </c>
-      <c r="H6" s="38">
-        <v>890</v>
-      </c>
-      <c r="I6" s="39">
-        <v>860</v>
-      </c>
-      <c r="J6" s="39">
-        <v>757</v>
-      </c>
-      <c r="K6" s="39">
-        <v>603</v>
-      </c>
-      <c r="L6" s="39">
-        <v>419</v>
-      </c>
-      <c r="M6" s="39">
-        <v>365</v>
-      </c>
-      <c r="N6" s="39">
-        <v>163</v>
-      </c>
-      <c r="O6" s="39">
-        <v>831</v>
-      </c>
-      <c r="P6" s="39">
-        <v>738</v>
+      <c r="A6" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="32">
+        <v>3230</v>
+      </c>
+      <c r="C6" s="32">
+        <v>3459</v>
+      </c>
+      <c r="D6" s="32">
+        <v>3697</v>
+      </c>
+      <c r="E6" s="32">
+        <v>3733</v>
+      </c>
+      <c r="F6" s="32">
+        <v>4616</v>
+      </c>
+      <c r="G6" s="32">
+        <v>4696</v>
+      </c>
+      <c r="H6" s="32">
+        <v>4158</v>
+      </c>
+      <c r="I6" s="32">
+        <v>3732</v>
+      </c>
+      <c r="J6" s="32">
+        <v>3745</v>
+      </c>
+      <c r="K6" s="33">
+        <v>3286</v>
+      </c>
+      <c r="L6" s="33">
+        <v>3039</v>
+      </c>
+      <c r="M6" s="33">
+        <v>2503</v>
+      </c>
+      <c r="N6" s="33">
+        <v>1173</v>
+      </c>
+      <c r="O6" s="33">
+        <v>6162</v>
+      </c>
+      <c r="P6" s="33">
+        <v>6395</v>
       </c>
     </row>
     <row r="7" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="36">
-        <v>61.29</v>
-      </c>
-      <c r="C7" s="36">
-        <v>124.18</v>
-      </c>
-      <c r="D7" s="36">
-        <v>191</v>
-      </c>
-      <c r="E7" s="36">
-        <v>179.64</v>
-      </c>
-      <c r="F7" s="36">
-        <v>213.66</v>
-      </c>
-      <c r="G7" s="36">
-        <v>262.89</v>
-      </c>
-      <c r="H7" s="36">
-        <v>186.9</v>
-      </c>
-      <c r="I7" s="36">
-        <v>301</v>
-      </c>
-      <c r="J7" s="36">
-        <v>295.23</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="35">
+        <v>0</v>
+      </c>
+      <c r="C7" s="35">
+        <v>0</v>
+      </c>
+      <c r="D7" s="35">
+        <v>0</v>
+      </c>
+      <c r="E7" s="35">
+        <v>0</v>
+      </c>
+      <c r="F7" s="35">
+        <v>0</v>
+      </c>
+      <c r="G7" s="35">
+        <v>46.96</v>
+      </c>
+      <c r="H7" s="35">
+        <v>41.58</v>
+      </c>
+      <c r="I7" s="35">
+        <v>74.64</v>
+      </c>
+      <c r="J7" s="35">
+        <v>187.25</v>
       </c>
       <c r="K7" s="36">
-        <v>301.5</v>
+        <v>164.3</v>
       </c>
       <c r="L7" s="36">
-        <v>184.36</v>
+        <v>151.94999999999999</v>
       </c>
       <c r="M7" s="36">
-        <v>135.05000000000001</v>
+        <v>175.21</v>
       </c>
       <c r="N7" s="36">
-        <v>70.09</v>
+        <v>117.3</v>
       </c>
       <c r="O7" s="36">
-        <f>0.54*O6</f>
-        <v>448.74</v>
+        <f>0.1*O6</f>
+        <v>616.20000000000005</v>
       </c>
       <c r="P7" s="36">
-        <f>0.49*P6</f>
-        <v>361.62</v>
+        <f>0.08*P6</f>
+        <v>511.6</v>
       </c>
     </row>
     <row r="8" spans="1:1025" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -9164,13 +9171,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="30">
+        <v>0.24880382779999999</v>
+      </c>
+      <c r="C11" s="30">
+        <v>0.1052631579</v>
+      </c>
+      <c r="D11" s="30">
         <v>0.15789473679999999</v>
-      </c>
-      <c r="C11" s="30">
-        <v>0.24880382779999999</v>
-      </c>
-      <c r="D11" s="30">
-        <v>0.1052631579</v>
       </c>
       <c r="E11" s="28">
         <v>0.1071428571</v>
@@ -9232,6 +9239,56 @@
       </c>
       <c r="P13" s="25">
         <v>9.8938662489999996E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="41">
+        <v>717555</v>
+      </c>
+      <c r="C14" s="41">
+        <v>788109</v>
+      </c>
+      <c r="D14" s="41">
+        <v>834650</v>
+      </c>
+      <c r="E14" s="41">
+        <v>876869</v>
+      </c>
+      <c r="F14" s="41">
+        <v>866690</v>
+      </c>
+      <c r="G14" s="41">
+        <v>904668</v>
+      </c>
+      <c r="H14" s="41">
+        <v>901797</v>
+      </c>
+      <c r="I14" s="41">
+        <v>937806</v>
+      </c>
+      <c r="J14" s="41">
+        <v>982396</v>
+      </c>
+      <c r="K14" s="41">
+        <v>1083783</v>
+      </c>
+      <c r="L14" s="41">
+        <v>973020</v>
+      </c>
+      <c r="M14" s="41">
+        <v>1049066</v>
+      </c>
+      <c r="N14" s="41">
+        <v>1005895</v>
+      </c>
+      <c r="O14" s="41">
+        <v>953924</v>
+      </c>
+      <c r="P14" s="41">
+        <v>958682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more cost framework and made a few changes on datasheets
</commit_message>
<xml_diff>
--- a/DataSheet_cddep.xlsx
+++ b/DataSheet_cddep.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="39">
   <si>
     <t>Year</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Pneumonia prevalence</t>
+  </si>
+  <si>
+    <t>Pneumonia breakdown (PA,AB,KP,EA/C)</t>
+  </si>
+  <si>
+    <t>CBP prescribed to pneumonia</t>
   </si>
 </sst>
 </file>
@@ -6628,7 +6634,7 @@
   <dimension ref="A1:AMK14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9168,24 +9174,24 @@
     </row>
     <row r="11" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B11" s="30">
-        <v>0.24880382779999999</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="C11" s="30">
-        <v>0.1052631579</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="D11" s="30">
-        <v>0.15789473679999999</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="E11" s="28">
-        <v>0.1071428571</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B12" s="23">
         <v>0.18589</v>
@@ -9196,49 +9202,49 @@
         <v>33</v>
       </c>
       <c r="B13" s="23">
-        <v>5.116795146E-2</v>
+        <v>6.8223934999999999E-2</v>
       </c>
       <c r="C13" s="23">
-        <v>5.545251382E-2</v>
+        <v>7.3936685000000002E-2</v>
       </c>
       <c r="D13" s="23">
-        <v>6.4058763709999994E-2</v>
+        <v>8.5411685000000001E-2</v>
       </c>
       <c r="E13" s="23">
-        <v>6.3038341819999996E-2</v>
+        <v>8.4051122000000006E-2</v>
       </c>
       <c r="F13" s="23">
-        <v>6.9081833790000005E-2</v>
+        <v>9.2109112000000007E-2</v>
       </c>
       <c r="G13" s="23">
-        <v>7.2866838119999999E-2</v>
+        <v>9.7155783999999995E-2</v>
       </c>
       <c r="H13" s="23">
-        <v>8.1495325930000001E-2</v>
+        <v>0.108660435</v>
       </c>
       <c r="I13" s="23">
-        <v>8.2100477039999994E-2</v>
+        <v>0.109467303</v>
       </c>
       <c r="J13" s="23">
-        <v>8.4872943630000003E-2</v>
+        <v>0.113163925</v>
       </c>
       <c r="K13" s="23">
-        <v>8.1556849720000005E-2</v>
+        <v>0.108742466</v>
       </c>
       <c r="L13" s="23">
-        <v>9.3080891629999996E-2</v>
+        <v>0.124107856</v>
       </c>
       <c r="M13" s="23">
-        <v>9.1138155499999998E-2</v>
+        <v>0.12151754100000001</v>
       </c>
       <c r="N13" s="23">
-        <v>9.7227641840000004E-2</v>
+        <v>0.12963685599999999</v>
       </c>
       <c r="O13" s="25">
-        <v>9.4034273060000007E-2</v>
+        <v>0.125379031</v>
       </c>
       <c r="P13" s="25">
-        <v>9.8938662489999996E-2</v>
+        <v>0.131918217</v>
       </c>
     </row>
     <row r="14" spans="1:1025" x14ac:dyDescent="0.25">

</xml_diff>